<commit_message>
XLSX cells containing date values should respect shouldFormatDate option
Return the ISO 8601 date string directly if option is set
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/sheet_with_dates_and_times.xlsx
+++ b/tests/resources/xlsx/sheet_with_dates_and_times.xlsx
@@ -449,8 +449,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
@@ -458,10 +458,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="2" min="1" width="11.6640625"/>
+    <col customWidth="1" max="3" min="3" width="11.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="23.5"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -498,9 +498,26 @@
         <v>0.69681712962962961</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="d">
+        <v>1976-11-22T08:30:00.000</v>
+      </c>
+      <c r="B3" t="d">
+        <v>1976-11-22T08:30</v>
+      </c>
+      <c r="C3" t="d">
+        <v>1582-10-15</v>
+      </c>
+      <c r="D3" t="d">
+        <v>08:30:00</v>
+      </c>
+      <c r="E3" t="d">
+        <v>08:30</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
XLSX cells containing date values should respect shouldFormatDate option (#282)
Return the ISO 8601 date string directly if option is set
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/sheet_with_dates_and_times.xlsx
+++ b/tests/resources/xlsx/sheet_with_dates_and_times.xlsx
@@ -449,8 +449,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
@@ -458,10 +458,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="2" min="1" width="11.6640625"/>
+    <col customWidth="1" max="3" min="3" width="11.6640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="23.5"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -498,9 +498,26 @@
         <v>0.69681712962962961</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="d">
+        <v>1976-11-22T08:30:00.000</v>
+      </c>
+      <c r="B3" t="d">
+        <v>1976-11-22T08:30</v>
+      </c>
+      <c r="C3" t="d">
+        <v>1582-10-15</v>
+      </c>
+      <c r="D3" t="d">
+        <v>08:30:00</v>
+      </c>
+      <c r="E3" t="d">
+        <v>08:30</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>